<commit_message>
fix: mensaje de error al cargar archivos
</commit_message>
<xml_diff>
--- a/src/assets/files/Plantilla_Productos_Megabahia.xlsx
+++ b/src/assets/files/Plantilla_Productos_Megabahia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEX\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847CE77A-AB86-48DE-B413-A9B897831253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6596251D-C3DA-468B-A2FD-CC75C4985AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{1302195F-7ADD-471D-B357-81CA800FC48C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1302195F-7ADD-471D-B357-81CA800FC48C}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -167,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,15 +172,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="NivelFila_4" xfId="1" builtinId="1" iLevel="3"/>
@@ -522,21 +520,22 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="15" max="19" width="14.140625" customWidth="1"/>
-    <col min="20" max="30" width="14.28515625" customWidth="1"/>
-    <col min="31" max="31" width="27" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13" style="6" customWidth="1"/>
+    <col min="5" max="10" width="12.85546875" style="6" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="17" style="6" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="6"/>
+    <col min="15" max="19" width="14.140625" style="6" customWidth="1"/>
+    <col min="20" max="30" width="14.28515625" style="6" customWidth="1"/>
+    <col min="31" max="31" width="27" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
@@ -546,91 +545,91 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -641,105 +640,105 @@
       <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="2"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="4"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
     </row>
     <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="2"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="5"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
     </row>
     <row r="4" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="2"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="4"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>